<commit_message>
Fixed Lists of Recommended Factors
</commit_message>
<xml_diff>
--- a/data/WHO  Datasets.xlsx
+++ b/data/WHO  Datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\westo\Documents\College\BIO 465\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14276B85-EF4B-493D-9F08-CB58483D547D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6951A403-C159-4547-AB7E-C852AF638F3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5EAED6A7-51C8-45A1-94F9-8AA6561A13B9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="142">
   <si>
     <t>Factor</t>
   </si>
@@ -442,6 +442,24 @@
   </si>
   <si>
     <t>Drop:</t>
+  </si>
+  <si>
+    <t>Use:</t>
+  </si>
+  <si>
+    <t>bcgv</t>
+  </si>
+  <si>
+    <t>dtpv</t>
+  </si>
+  <si>
+    <t>fullv</t>
+  </si>
+  <si>
+    <t>mslv</t>
+  </si>
+  <si>
+    <t>poliov</t>
   </si>
 </sst>
 </file>
@@ -802,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D74266D-91D3-45A2-97D0-212DBC11DFFC}">
-  <dimension ref="A2:M63"/>
+  <dimension ref="A2:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="94" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,7 +833,7 @@
     <col min="5" max="5" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -835,7 +853,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -852,7 +870,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -869,7 +887,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -886,7 +904,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -903,7 +921,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -920,7 +938,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -939,8 +957,11 @@
       <c r="M8" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P8" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -957,10 +978,13 @@
         <v>129</v>
       </c>
       <c r="M9" t="s">
+        <v>137</v>
+      </c>
+      <c r="P9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -977,10 +1001,13 @@
         <v>128</v>
       </c>
       <c r="M10" t="s">
+        <v>138</v>
+      </c>
+      <c r="P10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -997,10 +1024,13 @@
         <v>130</v>
       </c>
       <c r="M11" t="s">
+        <v>139</v>
+      </c>
+      <c r="P11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -1017,10 +1047,13 @@
         <v>128</v>
       </c>
       <c r="M12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -1037,10 +1070,13 @@
         <v>114</v>
       </c>
       <c r="M13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="P13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -1059,8 +1095,11 @@
       <c r="M14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -1079,8 +1118,11 @@
       <c r="M15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1099,8 +1141,11 @@
       <c r="M16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1119,8 +1164,11 @@
       <c r="M17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -1139,8 +1187,11 @@
       <c r="M18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -1159,8 +1210,11 @@
       <c r="M19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -1179,8 +1233,11 @@
       <c r="M20" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -1199,8 +1256,11 @@
       <c r="M21" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>3</v>
       </c>
@@ -1219,8 +1279,11 @@
       <c r="M22" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -1237,10 +1300,13 @@
         <v>128</v>
       </c>
       <c r="M23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="P23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -1257,10 +1323,13 @@
         <v>114</v>
       </c>
       <c r="M24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="P24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>3</v>
       </c>
@@ -1276,8 +1345,14 @@
       <c r="F25" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>88</v>
+      </c>
+      <c r="P25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -1293,8 +1368,11 @@
       <c r="F26" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -1310,8 +1388,11 @@
       <c r="F27" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>3</v>
       </c>
@@ -1327,8 +1408,11 @@
       <c r="F28" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -1344,8 +1428,11 @@
       <c r="F29" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -1361,8 +1448,11 @@
       <c r="F30" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>3</v>
       </c>
@@ -1378,8 +1468,11 @@
       <c r="F31" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>3</v>
       </c>
@@ -1395,8 +1488,11 @@
       <c r="F32" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>3</v>
       </c>
@@ -1412,8 +1508,11 @@
       <c r="F33" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>3</v>
       </c>
@@ -1429,8 +1528,11 @@
       <c r="F34" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>3</v>
       </c>
@@ -1446,8 +1548,11 @@
       <c r="F35" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -1463,8 +1568,11 @@
       <c r="F36" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>3</v>
       </c>
@@ -1480,8 +1588,11 @@
       <c r="F37" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>3</v>
       </c>
@@ -1497,8 +1608,11 @@
       <c r="F38" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1517,8 +1631,11 @@
       <c r="F39" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -1534,8 +1651,11 @@
       <c r="F40" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>3</v>
       </c>
@@ -1551,8 +1671,11 @@
       <c r="F41" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>3</v>
       </c>
@@ -1568,8 +1691,11 @@
       <c r="F42" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="P42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1712,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>3</v>
       </c>
@@ -1603,7 +1729,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>3</v>
       </c>
@@ -1620,7 +1746,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>3</v>
       </c>
@@ -1637,7 +1763,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>3</v>
       </c>
@@ -1654,7 +1780,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>3</v>
       </c>

</xml_diff>